<commit_message>
M3 QA Cord #282 - Implements Cord Test Data #242   - Add COA2.xlsx and COA3.xlsx
</commit_message>
<xml_diff>
--- a/05.Controls/M3.QA.Controls/Resources/Excels/COA4.xlsx
+++ b/05.Controls/M3.QA.Controls/Resources/Excels/COA4.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Toray Textiles (Thailand) Public Company Limited  Mill 3</t>
   </si>
@@ -78,9 +78,6 @@
     <t>MOISTURE REGAIN</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>ISSUED  BY</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>FINENESS</t>
+  </si>
+  <si>
+    <t>Date :</t>
   </si>
 </sst>
 </file>
@@ -158,8 +158,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="[$-1010409]d\ mmm\ yy;@"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="[$-1010409]d\ mmm\ yy;@"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -599,10 +599,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -614,7 +614,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -627,7 +627,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -671,97 +671,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -776,13 +689,100 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="4" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="5" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="5" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -839,7 +839,7 @@
         <xdr:cNvPr id="2" name="Line 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1FEA6510-7564-443B-BE4E-D29A1570EC84}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FEA6510-7564-443B-BE4E-D29A1570EC84}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -886,7 +886,7 @@
         <xdr:cNvPr id="3" name="Line 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4EC70211-43A7-4183-8A04-3D43485F5D7F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EC70211-43A7-4183-8A04-3D43485F5D7F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -933,7 +933,7 @@
         <xdr:cNvPr id="4" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D52C51D8-4719-4F50-B59F-C1824A264A67}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D52C51D8-4719-4F50-B59F-C1824A264A67}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1259,7 +1259,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1269,8 +1269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7:O7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="19.8"/>
@@ -1293,48 +1293,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.399999999999999">
-      <c r="S1" s="94"/>
+      <c r="S1" s="67"/>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="95"/>
+      <c r="S2" s="68"/>
     </row>
     <row r="3" spans="1:23" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="95"/>
+      <c r="S3" s="68"/>
     </row>
     <row r="4" spans="1:23" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="S4" s="95"/>
+      <c r="S4" s="68"/>
     </row>
     <row r="5" spans="1:23" ht="14.25" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="S5" s="95"/>
+      <c r="S5" s="68"/>
     </row>
     <row r="6" spans="1:23" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S6" s="95"/>
+      <c r="S6" s="68"/>
     </row>
     <row r="7" spans="1:23" ht="24" customHeight="1">
-      <c r="M7" s="78">
+      <c r="L7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M7" s="75">
         <v>44895</v>
       </c>
-      <c r="N7" s="78"/>
-      <c r="O7" s="78"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
     </row>
     <row r="8" spans="1:23" ht="33" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1350,35 +1353,35 @@
       <c r="M8" s="8"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
-      <c r="S8" s="101"/>
-      <c r="T8" s="101"/>
-      <c r="U8" s="101"/>
-      <c r="V8" s="101"/>
-      <c r="W8" s="101"/>
+      <c r="S8" s="72"/>
+      <c r="T8" s="72"/>
+      <c r="U8" s="72"/>
+      <c r="V8" s="72"/>
+      <c r="W8" s="72"/>
     </row>
     <row r="9" spans="1:23" ht="30" customHeight="1">
       <c r="L9" s="9"/>
-      <c r="P9" s="79"/>
-      <c r="Q9" s="79"/>
-      <c r="R9" s="96"/>
-      <c r="S9" s="98"/>
-      <c r="T9" s="101"/>
-      <c r="U9" s="101"/>
-      <c r="V9" s="101"/>
-      <c r="W9" s="101"/>
+      <c r="P9" s="76"/>
+      <c r="Q9" s="76"/>
+      <c r="R9" s="77"/>
+      <c r="S9" s="69"/>
+      <c r="T9" s="72"/>
+      <c r="U9" s="72"/>
+      <c r="V9" s="72"/>
+      <c r="W9" s="72"/>
     </row>
     <row r="10" spans="1:23" s="17" customFormat="1" ht="24.75" customHeight="1">
       <c r="A10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>25</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>26</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="12"/>
       <c r="F10" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="14" t="s">
@@ -1387,7 +1390,7 @@
       <c r="I10" s="14"/>
       <c r="J10" s="15"/>
       <c r="K10" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L10" s="11"/>
       <c r="M10" s="14"/>
@@ -1395,13 +1398,13 @@
         <v>22121</v>
       </c>
       <c r="O10" s="12"/>
-      <c r="Q10" s="80"/>
-      <c r="R10" s="97"/>
-      <c r="S10" s="99"/>
-      <c r="T10" s="99"/>
-      <c r="U10" s="99"/>
-      <c r="V10" s="99"/>
-      <c r="W10" s="99"/>
+      <c r="Q10" s="78"/>
+      <c r="R10" s="79"/>
+      <c r="S10" s="70"/>
+      <c r="T10" s="70"/>
+      <c r="U10" s="70"/>
+      <c r="V10" s="70"/>
+      <c r="W10" s="70"/>
     </row>
     <row r="11" spans="1:23" s="17" customFormat="1" ht="27.15" customHeight="1">
       <c r="A11" s="18"/>
@@ -1418,23 +1421,23 @@
       <c r="L11" s="19"/>
       <c r="M11" s="19"/>
       <c r="P11" s="20"/>
-      <c r="S11" s="100"/>
-      <c r="T11" s="100"/>
-      <c r="U11" s="100"/>
-      <c r="V11" s="100"/>
-      <c r="W11" s="100"/>
+      <c r="S11" s="71"/>
+      <c r="T11" s="71"/>
+      <c r="U11" s="71"/>
+      <c r="V11" s="71"/>
+      <c r="W11" s="71"/>
     </row>
     <row r="12" spans="1:23" s="17" customFormat="1" ht="18" customHeight="1">
       <c r="A12" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
-      <c r="D12" s="81" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="82"/>
-      <c r="F12" s="83"/>
+      <c r="D12" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="81"/>
+      <c r="F12" s="82"/>
       <c r="G12" s="23" t="s">
         <v>11</v>
       </c>
@@ -1444,11 +1447,11 @@
       <c r="K12" s="24"/>
       <c r="L12" s="22"/>
       <c r="M12" s="25"/>
-      <c r="N12" s="84" t="s">
-        <v>30</v>
-      </c>
-      <c r="O12" s="84" t="s">
-        <v>22</v>
+      <c r="N12" s="83" t="s">
+        <v>29</v>
+      </c>
+      <c r="O12" s="83" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:23" s="17" customFormat="1" ht="13.5" customHeight="1">
@@ -1459,28 +1462,28 @@
       <c r="E13" s="29"/>
       <c r="F13" s="30"/>
       <c r="G13" s="31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H13" s="24"/>
       <c r="I13" s="24"/>
       <c r="J13" s="24"/>
       <c r="K13" s="24"/>
-      <c r="L13" s="87" t="s">
-        <v>18</v>
-      </c>
-      <c r="M13" s="89" t="s">
-        <v>21</v>
-      </c>
-      <c r="N13" s="85"/>
-      <c r="O13" s="85"/>
+      <c r="L13" s="86" t="s">
+        <v>17</v>
+      </c>
+      <c r="M13" s="88" t="s">
+        <v>20</v>
+      </c>
+      <c r="N13" s="84"/>
+      <c r="O13" s="84"/>
     </row>
     <row r="14" spans="1:23" s="17" customFormat="1" ht="16.5" customHeight="1">
       <c r="A14" s="32"/>
       <c r="B14" s="19"/>
       <c r="C14" s="33"/>
-      <c r="D14" s="91"/>
-      <c r="E14" s="92"/>
-      <c r="F14" s="93"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="91"/>
+      <c r="F14" s="92"/>
       <c r="G14" s="34">
         <f>S10</f>
         <v>0</v>
@@ -1501,10 +1504,10 @@
         <f>W10</f>
         <v>0</v>
       </c>
-      <c r="L14" s="88"/>
-      <c r="M14" s="90"/>
-      <c r="N14" s="86"/>
-      <c r="O14" s="86"/>
+      <c r="L14" s="87"/>
+      <c r="M14" s="89"/>
+      <c r="N14" s="85"/>
+      <c r="O14" s="85"/>
     </row>
     <row r="15" spans="1:23" s="17" customFormat="1" ht="26.25" customHeight="1">
       <c r="A15" s="35" t="s">
@@ -1512,31 +1515,20 @@
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="72"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="74"/>
+        <v>31</v>
+      </c>
+      <c r="D15" s="93"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="95"/>
       <c r="G15" s="37"/>
       <c r="H15" s="37"/>
       <c r="I15" s="37"/>
       <c r="J15" s="37"/>
       <c r="K15" s="37"/>
-      <c r="L15" s="38" t="e">
-        <f t="shared" ref="L15:L23" si="0">AVERAGE(G15:K15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M15" s="39" t="e">
-        <f t="shared" ref="M15:M23" si="1">STDEV(G15:K15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N15" s="40" t="e">
-        <f>(L15-F15)/(3*M15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O15" s="41" t="s">
-        <v>15</v>
-      </c>
+      <c r="L15" s="38"/>
+      <c r="M15" s="39"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="41"/>
     </row>
     <row r="16" spans="1:23" s="17" customFormat="1" ht="26.25" customHeight="1">
       <c r="A16" s="35" t="s">
@@ -1544,192 +1536,125 @@
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="72"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="74"/>
+        <v>32</v>
+      </c>
+      <c r="D16" s="93"/>
+      <c r="E16" s="94"/>
+      <c r="F16" s="95"/>
       <c r="G16" s="37"/>
       <c r="H16" s="37"/>
       <c r="I16" s="37"/>
       <c r="J16" s="37"/>
       <c r="K16" s="37"/>
-      <c r="L16" s="42" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M16" s="43" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N16" s="40" t="e">
-        <f>(L16-F16)/(3*M16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O16" s="40" t="s">
-        <v>15</v>
-      </c>
+      <c r="L16" s="42"/>
+      <c r="M16" s="43"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="40"/>
     </row>
     <row r="17" spans="1:26" s="17" customFormat="1" ht="26.25" customHeight="1">
       <c r="A17" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="45"/>
       <c r="C17" s="46" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="72"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="74"/>
+        <v>32</v>
+      </c>
+      <c r="D17" s="93"/>
+      <c r="E17" s="94"/>
+      <c r="F17" s="95"/>
       <c r="G17" s="37"/>
       <c r="H17" s="37"/>
       <c r="I17" s="37"/>
       <c r="J17" s="37"/>
       <c r="K17" s="37"/>
-      <c r="L17" s="42" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M17" s="43" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N17" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="O17" s="40" t="s">
-        <v>15</v>
-      </c>
+      <c r="L17" s="42"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="40"/>
+      <c r="O17" s="40"/>
     </row>
     <row r="18" spans="1:26" s="17" customFormat="1" ht="26.25" customHeight="1">
       <c r="A18" s="35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="104"/>
-      <c r="E18" s="105"/>
-      <c r="F18" s="106"/>
+        <v>35</v>
+      </c>
+      <c r="D18" s="101"/>
+      <c r="E18" s="102"/>
+      <c r="F18" s="103"/>
       <c r="G18" s="47"/>
       <c r="H18" s="37"/>
       <c r="I18" s="37"/>
       <c r="J18" s="37"/>
       <c r="K18" s="37"/>
-      <c r="L18" s="42" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M18" s="43" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N18" s="40" t="e">
-        <f>F18*2/(6*M18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O18" s="40" t="e">
-        <f>N18*(1-((D18-L18)/F18))</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="L18" s="42"/>
+      <c r="M18" s="43"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="40"/>
     </row>
     <row r="19" spans="1:26" s="17" customFormat="1" ht="26.25" customHeight="1">
       <c r="A19" s="35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="48" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="104"/>
-      <c r="E19" s="105"/>
-      <c r="F19" s="106"/>
+        <v>35</v>
+      </c>
+      <c r="D19" s="101"/>
+      <c r="E19" s="102"/>
+      <c r="F19" s="103"/>
       <c r="G19" s="47"/>
       <c r="H19" s="37"/>
       <c r="I19" s="37"/>
       <c r="J19" s="37"/>
       <c r="K19" s="37"/>
-      <c r="L19" s="42" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M19" s="43" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N19" s="40" t="e">
-        <f>F19*2/(6*M19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O19" s="40" t="e">
-        <f>N19*(1-((D19-L19)/F19))</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="L19" s="42"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
     </row>
     <row r="20" spans="1:26" s="17" customFormat="1" ht="26.25" customHeight="1">
       <c r="A20" s="49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="50"/>
       <c r="C20" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="72"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="74"/>
+        <v>32</v>
+      </c>
+      <c r="D20" s="93"/>
+      <c r="E20" s="94"/>
+      <c r="F20" s="95"/>
       <c r="G20" s="37"/>
       <c r="H20" s="37"/>
       <c r="I20" s="37"/>
       <c r="J20" s="37"/>
       <c r="K20" s="37"/>
-      <c r="L20" s="42" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M20" s="43" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N20" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="O20" s="40" t="s">
-        <v>15</v>
-      </c>
+      <c r="L20" s="42"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="40"/>
     </row>
     <row r="21" spans="1:26" s="17" customFormat="1" ht="26.25" customHeight="1">
       <c r="A21" s="49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="50"/>
       <c r="C21" s="51" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="104"/>
-      <c r="E21" s="105"/>
-      <c r="F21" s="106"/>
+        <v>31</v>
+      </c>
+      <c r="D21" s="101"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="103"/>
       <c r="G21" s="37"/>
       <c r="H21" s="37"/>
       <c r="I21" s="37"/>
       <c r="J21" s="37"/>
       <c r="K21" s="37"/>
-      <c r="L21" s="42" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M21" s="43" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N21" s="40" t="e">
-        <f>F21*2/(6*M21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O21" s="40" t="e">
-        <f>N21*(1-((D21-L21)/F21))</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="L21" s="42"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
       <c r="S21" s="17" t="s">
         <v>10</v>
       </c>
@@ -1740,113 +1665,92 @@
       </c>
       <c r="B22" s="50"/>
       <c r="C22" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="102"/>
-      <c r="E22" s="103"/>
+        <v>32</v>
+      </c>
+      <c r="D22" s="73"/>
+      <c r="E22" s="74"/>
       <c r="F22" s="52"/>
       <c r="G22" s="43"/>
       <c r="H22" s="43"/>
       <c r="I22" s="43"/>
       <c r="J22" s="43"/>
       <c r="K22" s="43"/>
-      <c r="L22" s="53" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M22" s="43" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N22" s="40" t="e">
-        <f>(F22-L22)/(3*M22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O22" s="40" t="s">
-        <v>15</v>
-      </c>
+      <c r="L22" s="53"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="40"/>
+      <c r="O22" s="40"/>
     </row>
     <row r="23" spans="1:26" s="17" customFormat="1" ht="26.25" customHeight="1">
       <c r="A23" s="35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="72"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="74"/>
+        <v>19</v>
+      </c>
+      <c r="D23" s="93"/>
+      <c r="E23" s="94"/>
+      <c r="F23" s="95"/>
       <c r="G23" s="54"/>
       <c r="H23" s="54"/>
       <c r="I23" s="54"/>
       <c r="J23" s="54"/>
       <c r="K23" s="48"/>
-      <c r="L23" s="55" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M23" s="43" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N23" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="O23" s="40" t="s">
-        <v>15</v>
-      </c>
+      <c r="L23" s="55"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="40"/>
+      <c r="O23" s="40"/>
     </row>
     <row r="24" spans="1:26" s="17" customFormat="1" ht="21" customHeight="1"/>
     <row r="25" spans="1:26" s="17" customFormat="1" ht="16.5" customHeight="1">
-      <c r="J25" s="75" t="s">
+      <c r="J25" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="K25" s="76"/>
-      <c r="L25" s="76"/>
-      <c r="M25" s="77"/>
-      <c r="N25" s="70" t="s">
+      <c r="K25" s="97"/>
+      <c r="L25" s="97"/>
+      <c r="M25" s="98"/>
+      <c r="N25" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="O25" s="71"/>
+      <c r="O25" s="100"/>
     </row>
     <row r="26" spans="1:26" s="17" customFormat="1" ht="30" customHeight="1">
-      <c r="J26" s="20" t="e">
+      <c r="J26" s="20" t="str">
         <f>IF(L15&gt;F15,+"","NO PASSED")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K26" s="17" t="e">
+        <v>NO PASSED</v>
+      </c>
+      <c r="K26" s="17" t="str">
         <f>+IF(OR(L17&lt;(D17-F17),L17&gt;(D17+F17)),+"NO PASSED","")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L26" s="17" t="e">
+        <v/>
+      </c>
+      <c r="L26" s="17" t="str">
         <f>+IF(OR(L19&lt;(D19-F19),L19&gt;(D19+F19)),+"NO PASSED","")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M26" s="56" t="e">
+        <v/>
+      </c>
+      <c r="M26" s="56" t="str">
         <f>+IF(OR(L21&lt;(D21-F21),L21&gt;(D21+F21)),+"NO PASSED","")</f>
-        <v>#DIV/0!</v>
+        <v/>
       </c>
       <c r="N26" s="57"/>
       <c r="O26" s="58"/>
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" s="17" customFormat="1" ht="30" customHeight="1">
-      <c r="J27" s="59" t="e">
+      <c r="J27" s="59" t="str">
         <f>IF(L16&gt;F16,+"","NO PASSED")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K27" s="17" t="e">
+        <v>NO PASSED</v>
+      </c>
+      <c r="K27" s="17" t="str">
         <f>+IF(OR(L18&lt;(D18-F18),L18&gt;(D18+F18)),+"NO PASSED","")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L27" s="17" t="e">
+        <v/>
+      </c>
+      <c r="L27" s="17" t="str">
         <f>+IF(OR(L20&lt;(D20-F20),L20&gt;(D20+F20)),+"NO PASSED","")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M27" s="50" t="e">
+        <v/>
+      </c>
+      <c r="M27" s="50" t="str">
         <f>IF(L22&lt;F22,+"","NO PASSED")</f>
-        <v>#DIV/0!</v>
+        <v>NO PASSED</v>
       </c>
       <c r="N27" s="60"/>
       <c r="O27" s="61"/>
@@ -1860,31 +1764,31 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" s="17" customFormat="1">
-      <c r="J28" s="68" t="s">
+      <c r="J28" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="K28" s="69"/>
-      <c r="L28" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="M28" s="71"/>
+      <c r="K28" s="105"/>
+      <c r="L28" s="99" t="s">
+        <v>18</v>
+      </c>
+      <c r="M28" s="100"/>
       <c r="N28" s="23" t="s">
         <v>9</v>
       </c>
       <c r="O28" s="62"/>
-      <c r="R28" s="67"/>
-      <c r="S28" s="67"/>
-      <c r="T28" s="67"/>
-      <c r="U28" s="67"/>
-      <c r="V28" s="67"/>
-      <c r="W28" s="67"/>
-      <c r="X28" s="67"/>
+      <c r="R28" s="106"/>
+      <c r="S28" s="106"/>
+      <c r="T28" s="106"/>
+      <c r="U28" s="106"/>
+      <c r="V28" s="106"/>
+      <c r="W28" s="106"/>
+      <c r="X28" s="106"/>
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="51" customHeight="1">
       <c r="A29" s="63" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D29" s="64"/>
       <c r="J29" s="31"/>
@@ -1893,27 +1797,22 @@
       <c r="M29" s="65"/>
       <c r="N29" s="31"/>
       <c r="O29" s="66"/>
-      <c r="R29" s="67"/>
-      <c r="S29" s="67"/>
-      <c r="T29" s="67"/>
-      <c r="U29" s="67"/>
-      <c r="V29" s="67"/>
-      <c r="W29" s="67"/>
-      <c r="X29" s="67"/>
+      <c r="R29" s="106"/>
+      <c r="S29" s="106"/>
+      <c r="T29" s="106"/>
+      <c r="U29" s="106"/>
+      <c r="V29" s="106"/>
+      <c r="W29" s="106"/>
+      <c r="X29" s="106"/>
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="N12:N14"/>
-    <mergeCell ref="O12:O14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="R28:X28"/>
+    <mergeCell ref="R29:X29"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="J25:M25"/>
     <mergeCell ref="N25:O25"/>
@@ -1924,10 +1823,15 @@
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="D21:F21"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="R28:X28"/>
-    <mergeCell ref="R29:X29"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="N12:N14"/>
+    <mergeCell ref="O12:O14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="D14:F14"/>
   </mergeCells>
   <conditionalFormatting sqref="J26:M27">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>